<commit_message>
master music data file
</commit_message>
<xml_diff>
--- a/data/WORKING/pop_data.xlsx
+++ b/data/WORKING/pop_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/WORKING/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E6CE8A-1583-D447-86B3-F1DCD47FE521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD028ED-E8F1-F042-8350-24A5279C4877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10414,8 +10414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X875"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A875"/>
+    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
+      <selection sqref="A1:X875"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>